<commit_message>
outliers removed using iqr
</commit_message>
<xml_diff>
--- a/dataset1.xlsx
+++ b/dataset1.xlsx
@@ -355,8 +355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="K153" sqref="K153"/>
+    <sheetView tabSelected="1" topLeftCell="A429" workbookViewId="0">
+      <selection activeCell="G448" sqref="G448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2731,7 +2731,7 @@
         <v>6</v>
       </c>
       <c r="D173" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2745,7 +2745,7 @@
         <v>6</v>
       </c>
       <c r="D174" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2759,7 +2759,7 @@
         <v>6</v>
       </c>
       <c r="D175" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2773,7 +2773,7 @@
         <v>6</v>
       </c>
       <c r="D176" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2787,7 +2787,7 @@
         <v>6</v>
       </c>
       <c r="D177" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2815,7 +2815,7 @@
         <v>6</v>
       </c>
       <c r="D179" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2829,7 +2829,7 @@
         <v>6</v>
       </c>
       <c r="D180" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2843,7 +2843,7 @@
         <v>6</v>
       </c>
       <c r="D181" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2857,7 +2857,7 @@
         <v>6</v>
       </c>
       <c r="D182" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2871,7 +2871,7 @@
         <v>6</v>
       </c>
       <c r="D183" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2885,7 +2885,7 @@
         <v>6</v>
       </c>
       <c r="D184" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2899,7 +2899,7 @@
         <v>6</v>
       </c>
       <c r="D185" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2913,7 +2913,7 @@
         <v>6</v>
       </c>
       <c r="D186" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2927,7 +2927,7 @@
         <v>6</v>
       </c>
       <c r="D187" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2941,7 +2941,7 @@
         <v>6</v>
       </c>
       <c r="D188" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2955,7 +2955,7 @@
         <v>6</v>
       </c>
       <c r="D189" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2969,7 +2969,7 @@
         <v>6</v>
       </c>
       <c r="D190" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2983,7 +2983,7 @@
         <v>6</v>
       </c>
       <c r="D191" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2997,7 +2997,7 @@
         <v>6</v>
       </c>
       <c r="D192" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3011,7 +3011,7 @@
         <v>6</v>
       </c>
       <c r="D193" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3025,7 +3025,7 @@
         <v>6</v>
       </c>
       <c r="D194" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3039,7 +3039,7 @@
         <v>6</v>
       </c>
       <c r="D195" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3053,7 +3053,7 @@
         <v>6</v>
       </c>
       <c r="D196" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3067,7 +3067,7 @@
         <v>6</v>
       </c>
       <c r="D197" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3081,7 +3081,7 @@
         <v>6</v>
       </c>
       <c r="D198" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3095,7 +3095,7 @@
         <v>6</v>
       </c>
       <c r="D199" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3109,7 +3109,7 @@
         <v>6</v>
       </c>
       <c r="D200" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3123,7 +3123,7 @@
         <v>6</v>
       </c>
       <c r="D201" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3137,7 +3137,7 @@
         <v>6</v>
       </c>
       <c r="D202" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3151,7 +3151,7 @@
         <v>6</v>
       </c>
       <c r="D203" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3165,7 +3165,7 @@
         <v>6</v>
       </c>
       <c r="D204" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3179,7 +3179,7 @@
         <v>6</v>
       </c>
       <c r="D205" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3193,7 +3193,7 @@
         <v>6</v>
       </c>
       <c r="D206" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3207,7 +3207,7 @@
         <v>6</v>
       </c>
       <c r="D207" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3221,7 +3221,7 @@
         <v>6</v>
       </c>
       <c r="D208" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3235,7 +3235,7 @@
         <v>6</v>
       </c>
       <c r="D209" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3249,7 +3249,7 @@
         <v>6</v>
       </c>
       <c r="D210" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3263,7 +3263,7 @@
         <v>6</v>
       </c>
       <c r="D211" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4761,7 +4761,7 @@
         <v>6</v>
       </c>
       <c r="D318" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4775,7 +4775,7 @@
         <v>6</v>
       </c>
       <c r="D319" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4789,7 +4789,7 @@
         <v>6</v>
       </c>
       <c r="D320" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4803,7 +4803,7 @@
         <v>6</v>
       </c>
       <c r="D321" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4817,7 +4817,7 @@
         <v>6</v>
       </c>
       <c r="D322" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4831,7 +4831,7 @@
         <v>6</v>
       </c>
       <c r="D323" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4845,7 +4845,7 @@
         <v>6</v>
       </c>
       <c r="D324" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4859,7 +4859,7 @@
         <v>6</v>
       </c>
       <c r="D325" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="326" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4873,7 +4873,7 @@
         <v>6</v>
       </c>
       <c r="D326" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="327" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4887,7 +4887,7 @@
         <v>6</v>
       </c>
       <c r="D327" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4901,7 +4901,7 @@
         <v>6</v>
       </c>
       <c r="D328" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4915,7 +4915,7 @@
         <v>6</v>
       </c>
       <c r="D329" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4929,7 +4929,7 @@
         <v>6</v>
       </c>
       <c r="D330" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4943,7 +4943,7 @@
         <v>6</v>
       </c>
       <c r="D331" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4957,7 +4957,7 @@
         <v>6</v>
       </c>
       <c r="D332" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4971,7 +4971,7 @@
         <v>6</v>
       </c>
       <c r="D333" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4985,7 +4985,7 @@
         <v>6</v>
       </c>
       <c r="D334" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4999,7 +4999,7 @@
         <v>6</v>
       </c>
       <c r="D335" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5013,7 +5013,7 @@
         <v>6</v>
       </c>
       <c r="D336" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5027,7 +5027,7 @@
         <v>6</v>
       </c>
       <c r="D337" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5041,7 +5041,7 @@
         <v>6</v>
       </c>
       <c r="D338" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="339" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5055,7 +5055,7 @@
         <v>6</v>
       </c>
       <c r="D339" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="340" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5069,7 +5069,7 @@
         <v>6</v>
       </c>
       <c r="D340" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="341" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5083,7 +5083,7 @@
         <v>6</v>
       </c>
       <c r="D341" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5097,7 +5097,7 @@
         <v>6</v>
       </c>
       <c r="D342" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5111,7 +5111,7 @@
         <v>6</v>
       </c>
       <c r="D343" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="344" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5125,7 +5125,7 @@
         <v>6</v>
       </c>
       <c r="D344" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5139,7 +5139,7 @@
         <v>6</v>
       </c>
       <c r="D345" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="346" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5153,7 +5153,7 @@
         <v>6</v>
       </c>
       <c r="D346" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="347" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5167,7 +5167,7 @@
         <v>6</v>
       </c>
       <c r="D347" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="348" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5181,7 +5181,7 @@
         <v>6</v>
       </c>
       <c r="D348" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="349" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5195,7 +5195,7 @@
         <v>6</v>
       </c>
       <c r="D349" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5209,7 +5209,7 @@
         <v>6</v>
       </c>
       <c r="D350" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5223,7 +5223,7 @@
         <v>6</v>
       </c>
       <c r="D351" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5237,7 +5237,7 @@
         <v>6</v>
       </c>
       <c r="D352" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5251,7 +5251,7 @@
         <v>6</v>
       </c>
       <c r="D353" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="354" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5265,7 +5265,7 @@
         <v>6</v>
       </c>
       <c r="D354" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="355" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5279,7 +5279,7 @@
         <v>6</v>
       </c>
       <c r="D355" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="356" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5293,7 +5293,7 @@
         <v>6</v>
       </c>
       <c r="D356" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="357" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5307,7 +5307,7 @@
         <v>6</v>
       </c>
       <c r="D357" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="358" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5321,7 +5321,7 @@
         <v>6</v>
       </c>
       <c r="D358" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="359" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5335,7 +5335,7 @@
         <v>6</v>
       </c>
       <c r="D359" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="360" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5349,7 +5349,7 @@
         <v>6</v>
       </c>
       <c r="D360" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="361" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5363,7 +5363,7 @@
         <v>6</v>
       </c>
       <c r="D361" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="362" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5377,7 +5377,7 @@
         <v>6</v>
       </c>
       <c r="D362" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5391,7 +5391,7 @@
         <v>6</v>
       </c>
       <c r="D363" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="364" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5405,7 +5405,7 @@
         <v>6</v>
       </c>
       <c r="D364" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5419,7 +5419,7 @@
         <v>6</v>
       </c>
       <c r="D365" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5433,7 +5433,7 @@
         <v>6</v>
       </c>
       <c r="D366" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5447,7 +5447,7 @@
         <v>6</v>
       </c>
       <c r="D367" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5461,7 +5461,7 @@
         <v>6</v>
       </c>
       <c r="D368" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="369" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5475,7 +5475,7 @@
         <v>6</v>
       </c>
       <c r="D369" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="370" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5489,7 +5489,7 @@
         <v>6</v>
       </c>
       <c r="D370" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="371" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5503,7 +5503,7 @@
         <v>6</v>
       </c>
       <c r="D371" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="372" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5517,7 +5517,7 @@
         <v>6</v>
       </c>
       <c r="D372" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="373" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5531,7 +5531,7 @@
         <v>6</v>
       </c>
       <c r="D373" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="374" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5545,7 +5545,7 @@
         <v>6</v>
       </c>
       <c r="D374" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="375" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5559,7 +5559,7 @@
         <v>6</v>
       </c>
       <c r="D375" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="376" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5573,7 +5573,7 @@
         <v>6</v>
       </c>
       <c r="D376" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5587,7 +5587,7 @@
         <v>6</v>
       </c>
       <c r="D377" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="378" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5601,7 +5601,7 @@
         <v>6</v>
       </c>
       <c r="D378" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="379" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5615,7 +5615,7 @@
         <v>6</v>
       </c>
       <c r="D379" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="380" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5629,7 +5629,7 @@
         <v>6</v>
       </c>
       <c r="D380" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5643,7 +5643,7 @@
         <v>6</v>
       </c>
       <c r="D381" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5657,7 +5657,7 @@
         <v>6</v>
       </c>
       <c r="D382" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="383" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5671,7 +5671,7 @@
         <v>6</v>
       </c>
       <c r="D383" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="384" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5685,7 +5685,7 @@
         <v>6</v>
       </c>
       <c r="D384" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5699,7 +5699,7 @@
         <v>6</v>
       </c>
       <c r="D385" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="386" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5713,7 +5713,7 @@
         <v>6</v>
       </c>
       <c r="D386" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="387" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5727,7 +5727,7 @@
         <v>6</v>
       </c>
       <c r="D387" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="388" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5741,7 +5741,7 @@
         <v>6</v>
       </c>
       <c r="D388" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5755,7 +5755,7 @@
         <v>6</v>
       </c>
       <c r="D389" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="390" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5769,7 +5769,7 @@
         <v>6</v>
       </c>
       <c r="D390" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="391" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5783,7 +5783,7 @@
         <v>6</v>
       </c>
       <c r="D391" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5797,7 +5797,7 @@
         <v>6</v>
       </c>
       <c r="D392" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="393" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5811,7 +5811,7 @@
         <v>6</v>
       </c>
       <c r="D393" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5825,7 +5825,7 @@
         <v>6</v>
       </c>
       <c r="D394" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="395" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5839,7 +5839,7 @@
         <v>6</v>
       </c>
       <c r="D395" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="396" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5853,7 +5853,7 @@
         <v>6</v>
       </c>
       <c r="D396" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="397" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5867,7 +5867,7 @@
         <v>6</v>
       </c>
       <c r="D397" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="398" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5881,7 +5881,7 @@
         <v>6</v>
       </c>
       <c r="D398" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="399" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5895,7 +5895,7 @@
         <v>6</v>
       </c>
       <c r="D399" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5909,7 +5909,7 @@
         <v>6</v>
       </c>
       <c r="D400" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="401" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5923,7 +5923,7 @@
         <v>6</v>
       </c>
       <c r="D401" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="402" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5937,7 +5937,7 @@
         <v>6</v>
       </c>
       <c r="D402" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="403" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5951,7 +5951,7 @@
         <v>6</v>
       </c>
       <c r="D403" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="404" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5965,7 +5965,7 @@
         <v>6</v>
       </c>
       <c r="D404" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="405" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5979,7 +5979,7 @@
         <v>6</v>
       </c>
       <c r="D405" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="406" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5993,7 +5993,7 @@
         <v>6</v>
       </c>
       <c r="D406" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="407" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6007,7 +6007,7 @@
         <v>6</v>
       </c>
       <c r="D407" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="408" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6021,7 +6021,7 @@
         <v>6</v>
       </c>
       <c r="D408" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="409" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6035,7 +6035,7 @@
         <v>6</v>
       </c>
       <c r="D409" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="410" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6049,7 +6049,7 @@
         <v>6</v>
       </c>
       <c r="D410" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="411" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6063,7 +6063,7 @@
         <v>6</v>
       </c>
       <c r="D411" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="412" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6077,7 +6077,7 @@
         <v>6</v>
       </c>
       <c r="D412" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="413" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6091,7 +6091,7 @@
         <v>6</v>
       </c>
       <c r="D413" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6105,7 +6105,7 @@
         <v>6</v>
       </c>
       <c r="D414" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="415" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6119,7 +6119,7 @@
         <v>6</v>
       </c>
       <c r="D415" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="416" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6133,7 +6133,7 @@
         <v>6</v>
       </c>
       <c r="D416" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="417" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6147,7 +6147,7 @@
         <v>6</v>
       </c>
       <c r="D417" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="418" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6161,7 +6161,7 @@
         <v>6</v>
       </c>
       <c r="D418" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="419" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6175,7 +6175,7 @@
         <v>6</v>
       </c>
       <c r="D419" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="420" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6189,7 +6189,7 @@
         <v>6</v>
       </c>
       <c r="D420" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="421" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6203,7 +6203,7 @@
         <v>6</v>
       </c>
       <c r="D421" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="422" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6217,7 +6217,7 @@
         <v>6</v>
       </c>
       <c r="D422" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="423" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6231,7 +6231,7 @@
         <v>6</v>
       </c>
       <c r="D423" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6245,7 +6245,7 @@
         <v>6</v>
       </c>
       <c r="D424" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="425" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6259,7 +6259,7 @@
         <v>6</v>
       </c>
       <c r="D425" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="426" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6273,7 +6273,7 @@
         <v>6</v>
       </c>
       <c r="D426" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="427" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6287,7 +6287,7 @@
         <v>6</v>
       </c>
       <c r="D427" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="428" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6301,7 +6301,7 @@
         <v>6</v>
       </c>
       <c r="D428" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="429" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6315,7 +6315,7 @@
         <v>6</v>
       </c>
       <c r="D429" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6329,7 +6329,7 @@
         <v>6</v>
       </c>
       <c r="D430" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="431" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6343,7 +6343,7 @@
         <v>6</v>
       </c>
       <c r="D431" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6357,7 +6357,7 @@
         <v>6</v>
       </c>
       <c r="D432" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="433" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6371,7 +6371,7 @@
         <v>6</v>
       </c>
       <c r="D433" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="434" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6385,7 +6385,7 @@
         <v>6</v>
       </c>
       <c r="D434" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="435" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6399,7 +6399,7 @@
         <v>6</v>
       </c>
       <c r="D435" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="436" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6413,7 +6413,7 @@
         <v>6</v>
       </c>
       <c r="D436" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="437" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6427,7 +6427,7 @@
         <v>6</v>
       </c>
       <c r="D437" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="438" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6441,7 +6441,7 @@
         <v>6</v>
       </c>
       <c r="D438" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="439" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6455,7 +6455,7 @@
         <v>6</v>
       </c>
       <c r="D439" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="440" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6469,7 +6469,7 @@
         <v>6</v>
       </c>
       <c r="D440" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6483,7 +6483,7 @@
         <v>6</v>
       </c>
       <c r="D441" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="442" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6497,7 +6497,7 @@
         <v>6</v>
       </c>
       <c r="D442" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="443" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6511,7 +6511,7 @@
         <v>6</v>
       </c>
       <c r="D443" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="444" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6525,7 +6525,7 @@
         <v>6</v>
       </c>
       <c r="D444" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="445" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6539,7 +6539,7 @@
         <v>6</v>
       </c>
       <c r="D445" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="446" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6553,7 +6553,7 @@
         <v>6</v>
       </c>
       <c r="D446" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="447" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6567,7 +6567,7 @@
         <v>6</v>
       </c>
       <c r="D447" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="448" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6581,7 +6581,7 @@
         <v>6</v>
       </c>
       <c r="D448" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="449" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6595,7 +6595,7 @@
         <v>6</v>
       </c>
       <c r="D449" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6609,7 +6609,7 @@
         <v>6</v>
       </c>
       <c r="D450" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="451" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6623,7 +6623,7 @@
         <v>6</v>
       </c>
       <c r="D451" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="452" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6637,7 +6637,7 @@
         <v>6</v>
       </c>
       <c r="D452" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="453" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -6651,7 +6651,7 @@
         <v>6</v>
       </c>
       <c r="D453" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="454" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>